<commit_message>
Added defines for the torque and trust sensors
</commit_message>
<xml_diff>
--- a/TestJig/TESTS.xlsx
+++ b/TestJig/TESTS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>TEST NUMBER</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Voltage (V)</t>
+  </si>
+  <si>
+    <t>Room Temperature</t>
   </si>
 </sst>
 </file>
@@ -453,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7:L8"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,15 +477,15 @@
     <col min="17" max="17" width="32" customWidth="1"/>
     <col min="18" max="18" width="30.5703125" customWidth="1"/>
     <col min="20" max="20" width="22" customWidth="1"/>
-    <col min="22" max="22" width="20.28515625" customWidth="1"/>
-    <col min="23" max="23" width="6.42578125" customWidth="1"/>
-    <col min="24" max="24" width="13" customWidth="1"/>
-    <col min="25" max="25" width="19.5703125" customWidth="1"/>
-    <col min="26" max="26" width="18.140625" customWidth="1"/>
-    <col min="27" max="27" width="13.7109375" customWidth="1"/>
+    <col min="22" max="23" width="20.28515625" customWidth="1"/>
+    <col min="24" max="24" width="6.42578125" customWidth="1"/>
+    <col min="25" max="25" width="13" customWidth="1"/>
+    <col min="26" max="26" width="19.5703125" customWidth="1"/>
+    <col min="27" max="27" width="18.140625" customWidth="1"/>
+    <col min="28" max="28" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
@@ -520,8 +523,9 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -589,24 +593,27 @@
         <v>26</v>
       </c>
       <c r="W2" t="s">
+        <v>32</v>
+      </c>
+      <c r="X2" t="s">
         <v>27</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>28</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>30</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="S1:AA1"/>
+    <mergeCell ref="S1:AB1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="P1:R1"/>

</xml_diff>